<commit_message>
multi-line in Excel Export
</commit_message>
<xml_diff>
--- a/Extensions/Signum.Excel/plainExcelTemplate.xlsx
+++ b/Extensions/Signum.Excel/plainExcelTemplate.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Signum\southwind\Framework\Signum.Engine.Extensions\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\VdS\Framework\Extensions\Signum.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477A6F4C-E641-45FD-B2F8-0ADB0BDF64AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="5085" windowWidth="21600" windowHeight="12735"/>
+    <workbookView xWindow="28680" yWindow="-2625" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>HeaderCell</t>
   </si>
@@ -63,17 +53,29 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>Multiline</t>
+  </si>
+  <si>
+    <t>Apple
+Orange</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>Hallo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="[$¥-804]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0&quot; km&quot;"/>
     <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -143,22 +145,23 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -181,9 +184,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,9 +224,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,7 +261,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,7 +296,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,24 +469,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.6">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,76 +514,84 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="K2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>31361</v>
       </c>
       <c r="C3" s="3">
         <v>30278.40625</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="4">
         <v>12</v>
       </c>
       <c r="G3" s="5">
         <v>12</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>0.2</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="12">
         <v>0.5</v>
       </c>
-      <c r="J3" s="11" t="b">
+      <c r="J3" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L14" s="12"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L16" s="12"/>
+      <c r="K3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>